<commit_message>
exempt process emissions from carbon tax
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BEPEfCT/Boolean Exempt Process Emissions From Carbon Tax.xlsx
+++ b/InputData/ctrl-settings/BEPEfCT/Boolean Exempt Process Emissions From Carbon Tax.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/ctrl-settings/bepefct/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\ctrl-settings\BEPEfCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E6BF0F-B308-674A-8316-CAC8B2805AFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5567614-2D1D-478F-864A-A36FD9229755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="1140" windowWidth="24100" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4695" yWindow="1950" windowWidth="22980" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -441,11 +441,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -453,42 +455,42 @@
         <v>44307</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -506,21 +508,23 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add in AC2 and IRA files/policies
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BEPEfCT/Boolean Exempt Process Emissions From Carbon Tax.xlsx
+++ b/InputData/ctrl-settings/BEPEfCT/Boolean Exempt Process Emissions From Carbon Tax.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\ctrl-settings\BEPEfCT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ctrl-settings\BEPEfCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46ADB21C-4234-4425-B751-6BF6CB8F7A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6985757-BBE2-4903-9695-7087C0DE082D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12120" yWindow="2835" windowWidth="16515" windowHeight="13785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>This variable is a control lever.  A control lever is neither a policy nor input data.</t>
   </si>
@@ -35,9 +35,6 @@
     <t>country or use case, then left alone.</t>
   </si>
   <si>
-    <t>Boolean</t>
-  </si>
-  <si>
     <t>As a boolean lever, use "0" to cause process emissions (which are generated by</t>
   </si>
   <si>
@@ -54,13 +51,97 @@
   </si>
   <si>
     <t>BEPEfCT Boolean Exempt Process Emissions from Carbon Tax</t>
+  </si>
+  <si>
+    <t>agriculture and forestry 01T03</t>
+  </si>
+  <si>
+    <t>coal mining 05</t>
+  </si>
+  <si>
+    <t>oil and gas extraction 06</t>
+  </si>
+  <si>
+    <t>other mining and quarrying 07T08</t>
+  </si>
+  <si>
+    <t>food beverage and tobacco 10T12</t>
+  </si>
+  <si>
+    <t>textiles apparel and leather 13T15</t>
+  </si>
+  <si>
+    <t>wood products 16</t>
+  </si>
+  <si>
+    <t>pulp paper and printing 17T18</t>
+  </si>
+  <si>
+    <t>refined petroleum and coke 19</t>
+  </si>
+  <si>
+    <t>chemicals 20</t>
+  </si>
+  <si>
+    <t>rubber and plastic products 22</t>
+  </si>
+  <si>
+    <t>glass and glass products 231</t>
+  </si>
+  <si>
+    <t>cement and other nonmetallic minerals 239</t>
+  </si>
+  <si>
+    <t>iron and steel 241</t>
+  </si>
+  <si>
+    <t>other metals 242</t>
+  </si>
+  <si>
+    <t>metal products except machinery and vehicles 25</t>
+  </si>
+  <si>
+    <t>computers and electronics 26</t>
+  </si>
+  <si>
+    <t>appliances and electrical equipment 27</t>
+  </si>
+  <si>
+    <t>other machinery 28</t>
+  </si>
+  <si>
+    <t>road vehicles 29</t>
+  </si>
+  <si>
+    <t>nonroad vehicles 30</t>
+  </si>
+  <si>
+    <t>other manufacturing 31T33</t>
+  </si>
+  <si>
+    <t>energy pipelines and gas processing 352T353</t>
+  </si>
+  <si>
+    <t>water and waste 36T39</t>
+  </si>
+  <si>
+    <t>construction 41T43</t>
+  </si>
+  <si>
+    <t>Unit: boolean (0 or 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the U.S., we exempt agriculture and water and waste process emissions. Generally, </t>
+  </si>
+  <si>
+    <t>proposed taxes do not cover these sectors.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +151,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -100,7 +189,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,60 +528,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2">
-        <v>44307</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -506,28 +602,227 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="47.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>